<commit_message>
CSV Result in progress
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -160,6 +160,12 @@
   </si>
   <si>
     <t>https://www.londonstockexchange.com/</t>
+  </si>
+  <si>
+    <t>ResultFolderPath</t>
+  </si>
+  <si>
+    <t>C:\UiPath\Results</t>
   </si>
 </sst>
 </file>
@@ -535,7 +541,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -546,7 +552,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -631,7 +637,14 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>